<commit_message>
se arregla PAS 2302 en recording BusquedaDeCodigosDeProductor y se agrega ambiente QA en creación de Plan Autonomía
</commit_message>
<xml_diff>
--- a/CardaData/DataSource-CreacionPlanAutonomia.xlsx
+++ b/CardaData/DataSource-CreacionPlanAutonomia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Downloads\Sura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\CardaData\CardaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C67C75F6-EF0D-49B5-B692-A4EC635216ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E3185B-4503-4B21-AB3B-7EA26D707CEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{852C77DF-5F2B-4498-9C53-FC44E4116A48}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Ambiente</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>https://suragwqa2.segurossura.com.ar/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31914A1-BDA5-4316-AFCC-FB6C424C2FDF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,9 +457,24 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B6EDDB0F-E8F8-468D-9850-A24F9E94B71E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{EE2B2055-4364-4086-834E-A00E039BE076}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>